<commit_message>
fix: update equipos.xlsx filem con cadete b fase final
</commit_message>
<xml_diff>
--- a/equipos.xlsx
+++ b/equipos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\algog\Documents\Diseño Gráfico Coras\2024 - 2025\App Horarios 2425\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1538765-13EF-48E6-AF89-803DCEB6C4A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E95990A-04EB-4997-97E8-38DA02BA5B0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="2280" windowWidth="16200" windowHeight="9970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -106,9 +106,6 @@
     <t>CADETE F</t>
   </si>
   <si>
-    <t>https://www.rfebm.com/competiciones/resultados_completos.php?seleccion=0&amp;id=1027620</t>
-  </si>
-  <si>
     <t>CORAZONISTAS B  2CM</t>
   </si>
   <si>
@@ -182,6 +179,9 @@
   </si>
   <si>
     <t>https://www.rfebm.com/competiciones/competicion.php?seleccion=0&amp;id=1026965&amp;jornada=12&amp;id_ambito=0</t>
+  </si>
+  <si>
+    <t>https://www.rfebm.com/competiciones/resultados_completos.php?seleccion=0&amp;id=1028265</t>
   </si>
 </sst>
 </file>
@@ -261,13 +261,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -574,7 +575,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -636,7 +637,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -647,7 +648,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
@@ -690,95 +691,98 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="A11" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" t="s">
         <v>28</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>29</v>
-      </c>
-      <c r="C11" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
         <v>31</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>32</v>
-      </c>
-      <c r="C12" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
         <v>34</v>
-      </c>
-      <c r="C13" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" t="s">
         <v>36</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>37</v>
-      </c>
-      <c r="C14" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s">
         <v>39</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>40</v>
-      </c>
-      <c r="C15" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
         <v>42</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>43</v>
-      </c>
-      <c r="C16" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" t="s">
         <v>45</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>46</v>
-      </c>
-      <c r="C17" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" t="s">
         <v>48</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>49</v>
       </c>
-      <c r="C18" t="s">
-        <v>50</v>
-      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A11" r:id="rId1" xr:uid="{E4D29B5D-D815-4231-844B-AF6930A2DD29}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Actualizado 12-mar con nuevas fases
</commit_message>
<xml_diff>
--- a/equipos.xlsx
+++ b/equipos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\algog\Documents\Diseño Gráfico Coras\2024 - 2025\App Horarios 2425\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E95990A-04EB-4997-97E8-38DA02BA5B0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5929A38B-51FF-4E52-A8B1-832139692C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -79,9 +79,6 @@
     <t>INFANTIL F</t>
   </si>
   <si>
-    <t>https://www.rfebm.com/competiciones/resultados_completos.php?seleccion=0&amp;id=1026259</t>
-  </si>
-  <si>
     <t>CORAZONISTAS B  2I</t>
   </si>
   <si>
@@ -178,10 +175,13 @@
     <t>https://www.rfebm.com/competiciones/resultados_completos.php?seleccion=0&amp;id=1026059</t>
   </si>
   <si>
-    <t>https://www.rfebm.com/competiciones/competicion.php?seleccion=0&amp;id=1026965&amp;jornada=12&amp;id_ambito=0</t>
-  </si>
-  <si>
     <t>https://www.rfebm.com/competiciones/resultados_completos.php?seleccion=0&amp;id=1028265</t>
+  </si>
+  <si>
+    <t>https://www.rfebm.com/competiciones/competicion.php?seleccion=0&amp;id=1026965&amp;jornada=13&amp;id_ambito=0</t>
+  </si>
+  <si>
+    <t>https://www.rfebm.com/competiciones/resultados_completos.php?seleccion=0&amp;id=1028401</t>
   </si>
 </sst>
 </file>
@@ -572,15 +572,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -591,7 +591,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -602,7 +602,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -613,7 +613,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -624,7 +624,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -635,7 +635,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>52</v>
       </c>
@@ -646,9 +646,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
@@ -657,125 +657,126 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>20</v>
       </c>
-      <c r="C8" t="s">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
         <v>22</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>23</v>
       </c>
-      <c r="C9" t="s">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
         <v>25</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>26</v>
       </c>
-      <c r="C10" t="s">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>28</v>
       </c>
-      <c r="C11" t="s">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
         <v>30</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>31</v>
       </c>
-      <c r="C12" t="s">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>33</v>
       </c>
-      <c r="C13" t="s">
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
         <v>35</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>36</v>
       </c>
-      <c r="C14" t="s">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
         <v>38</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>39</v>
       </c>
-      <c r="C15" t="s">
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
         <v>41</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>42</v>
-      </c>
-      <c r="C16" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" t="s">
         <v>44</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>45</v>
-      </c>
-      <c r="C17" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" t="s">
         <v>47</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>48</v>
-      </c>
-      <c r="C18" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizado Fase Final Sen Fem
</commit_message>
<xml_diff>
--- a/equipos.xlsx
+++ b/equipos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\algog\Documents\Diseño Gráfico Coras\2024 - 2025\App Horarios 2425\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5929A38B-51FF-4E52-A8B1-832139692C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69ABD9FB-074A-499F-A378-41FAB34150CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -133,9 +134,6 @@
     <t>JUVENIL A</t>
   </si>
   <si>
-    <t>https://www.rfebm.com/competiciones/resultados_completos.php?seleccion=0&amp;id=1026246</t>
-  </si>
-  <si>
     <t>CORAZONISTAS B 2NF</t>
   </si>
   <si>
@@ -151,9 +149,6 @@
     <t>SENIOR MASC B</t>
   </si>
   <si>
-    <t>https://www.rfebm.com/competiciones/resultados_completos.php?seleccion=0&amp;id=1026245</t>
-  </si>
-  <si>
     <t>CORAZONISTAS A 2NF</t>
   </si>
   <si>
@@ -182,6 +177,12 @@
   </si>
   <si>
     <t>https://www.rfebm.com/competiciones/resultados_completos.php?seleccion=0&amp;id=1028401</t>
+  </si>
+  <si>
+    <t>https://www.rfebm.com/competiciones/resultados_completos.php?seleccion=0&amp;id=1028442</t>
+  </si>
+  <si>
+    <t>https://www.rfebm.com/competiciones/resultados_completos.php?seleccion=0&amp;id=1028443</t>
   </si>
 </sst>
 </file>
@@ -572,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -637,7 +638,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -648,7 +649,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
@@ -659,7 +660,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
@@ -692,7 +693,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B11" t="s">
         <v>27</v>
@@ -714,7 +715,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B13" t="s">
         <v>32</v>
@@ -736,48 +737,51 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" t="s">
         <v>37</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>38</v>
-      </c>
-      <c r="C15" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s">
         <v>40</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C17" t="s">
         <v>41</v>
       </c>
-      <c r="C16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" t="s">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>44</v>
       </c>
-      <c r="C17" t="s">
+      <c r="B18" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="C18" t="s">
         <v>46</v>
       </c>
-      <c r="B18" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" t="s">
-        <v>48</v>
-      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D19" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
fix: update equipos.xlsx file
</commit_message>
<xml_diff>
--- a/equipos.xlsx
+++ b/equipos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\algog\Documents\Diseño Gráfico Coras\2024 - 2025\App Horarios 2425\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2636EFA1-AA8B-426B-A7EF-3646D4AB924B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D7026D-6553-4153-8804-6D4AF26916E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="10980" windowHeight="13770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -73,9 +73,6 @@
     <t>INFANTIL B</t>
   </si>
   <si>
-    <t>https://www.rfebm.com/competiciones/resultados_completos.php?seleccion=0&amp;id=1024670</t>
-  </si>
-  <si>
     <t>CORAZONISTAS A 1IM</t>
   </si>
   <si>
@@ -97,9 +94,6 @@
     <t>CADETE B</t>
   </si>
   <si>
-    <t>https://www.rfebm.com/competiciones/resultados_completos.php?seleccion=0&amp;id=1024664</t>
-  </si>
-  <si>
     <t>CORAZONISTAS A 1CM</t>
   </si>
   <si>
@@ -112,9 +106,6 @@
     <t>JUVENIL B</t>
   </si>
   <si>
-    <t>https://www.rfebm.com/competiciones/resultados_completos.php?seleccion=0&amp;id=1024665</t>
-  </si>
-  <si>
     <t>CORAZONISTAS A 1JM</t>
   </si>
   <si>
@@ -157,12 +148,6 @@
     <t>https://www.rfebm.com/competiciones/resultados_completos.php?seleccion=0&amp;id=1026059</t>
   </si>
   <si>
-    <t>https://www.rfebm.com/competiciones/resultados_completos.php?seleccion=0&amp;id=1028265</t>
-  </si>
-  <si>
-    <t>https://www.rfebm.com/competiciones/resultados_completos.php?seleccion=0&amp;id=1028401</t>
-  </si>
-  <si>
     <t>https://www.rfebm.com/competiciones/resultados_completos.php?seleccion=0&amp;id=1028442</t>
   </si>
   <si>
@@ -182,6 +167,21 @@
   </si>
   <si>
     <t>https://www.rfebm.com/competiciones/competicion.php?seleccion=0&amp;id=1029312</t>
+  </si>
+  <si>
+    <t>https://www.rfebm.com/competiciones/resultados_completos.php?seleccion=0&amp;id=1029448</t>
+  </si>
+  <si>
+    <t>https://www.rfebm.com/competiciones/resultados_completos.php?seleccion=0&amp;id=1029449</t>
+  </si>
+  <si>
+    <t>https://www.rfebm.com/competiciones/resultados_completos.php?seleccion=0&amp;id=1029461</t>
+  </si>
+  <si>
+    <t>https://www.rfebm.com/competiciones/resultados_completos.php?seleccion=0&amp;id=1029465</t>
+  </si>
+  <si>
+    <t>https://www.rfebm.com/competiciones/resultados_completos.php?seleccion=0&amp;id=1029469</t>
   </si>
 </sst>
 </file>
@@ -575,7 +575,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -597,7 +597,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -608,7 +608,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -619,7 +619,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -630,7 +630,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
@@ -641,7 +641,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -652,7 +652,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
@@ -663,7 +663,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
@@ -674,113 +674,113 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" t="s">
         <v>17</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>18</v>
-      </c>
-      <c r="C9" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
         <v>20</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>21</v>
-      </c>
-      <c r="C10" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
         <v>23</v>
-      </c>
-      <c r="C11" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
         <v>25</v>
-      </c>
-      <c r="B12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
@@ -788,11 +788,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A11" r:id="rId1" xr:uid="{E4D29B5D-D815-4231-844B-AF6930A2DD29}"/>
-    <hyperlink ref="A4" r:id="rId2" xr:uid="{609FDFA9-CF54-4C04-B324-690EAFE06690}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{1ECC46DC-1FD1-4772-B50F-2425C891A82E}"/>
+    <hyperlink ref="A4" r:id="rId1" xr:uid="{609FDFA9-CF54-4C04-B324-690EAFE06690}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{1ECC46DC-1FD1-4772-B50F-2425C891A82E}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>